<commit_message>
* v1.0.5 Update analysis with credible set SNPs.
</commit_message>
<xml_diff>
--- a/SNP/Variants.xlsx
+++ b/SNP/Variants.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slaan3/OneDrive - UMC Utrecht/PLINK/analyses/lookups/AE_20200512_COL_MKAVOUSI_MBOS_CHARGE_1000G_CAC/SNP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umcutrecht-my.sharepoint.com/personal/s_w_vanderlaan-2_umcutrecht_nl/Documents/PLINK/analyses/lookups/AE_20200512_COL_MKAVOUSI_MBOS_CHARGE_1000G_CAC/SNP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E831D9C1-59D1-4846-9BB2-CA9DCE5F216B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{E831D9C1-59D1-4846-9BB2-CA9DCE5F216B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1D1F9E7-D81F-594E-A6C7-EBCBEF86C7DA}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="500" windowWidth="19340" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2260" yWindow="500" windowWidth="25540" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variants" sheetId="3" r:id="rId1"/>
+    <sheet name="CredibleSet" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variants!$A$1:$J$6</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4500" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5128" uniqueCount="981">
   <si>
     <t>single nucleotide variant</t>
   </si>
@@ -2931,6 +2932,54 @@
   </si>
   <si>
     <t>ACT</t>
+  </si>
+  <si>
+    <t>Posterior_Prob</t>
+  </si>
+  <si>
+    <t>rs10762577_locus_all</t>
+  </si>
+  <si>
+    <t>rs10899970_locus_all</t>
+  </si>
+  <si>
+    <t>rs6593394</t>
+  </si>
+  <si>
+    <t>rs10793513</t>
+  </si>
+  <si>
+    <t>rs11063120_locus_all</t>
+  </si>
+  <si>
+    <t>rs2854746_locus_all</t>
+  </si>
+  <si>
+    <t>rs3844006_locus_all</t>
+  </si>
+  <si>
+    <t>rs4977575_locus_all</t>
+  </si>
+  <si>
+    <t>rs7182103_locus_all</t>
+  </si>
+  <si>
+    <t>rs7412_locus_all</t>
+  </si>
+  <si>
+    <t>rs9349379_locus_all</t>
+  </si>
+  <si>
+    <t>rs9515203_locus_all</t>
+  </si>
+  <si>
+    <t>rs9633535_locus_all</t>
+  </si>
+  <si>
+    <t>rs10821952</t>
+  </si>
+  <si>
+    <t>rs10761603</t>
   </si>
 </sst>
 </file>
@@ -3265,8 +3314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F080AD-A6C4-C84A-8AC2-B8A18EFA85A7}">
   <dimension ref="A1:J899"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30251,4 +30300,3461 @@
   <autoFilter ref="A1:J6" xr:uid="{167C23E3-82A9-AE4E-9BE3-55938972511E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6C5C1E-F70F-D647-AB85-387F5EA1E1D9}">
+  <dimension ref="A1:J104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE(D2,":",E2)</f>
+        <v>10:75917431</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>75917431</v>
+      </c>
+      <c r="F2" t="s">
+        <v>912</v>
+      </c>
+      <c r="G2" t="s">
+        <v>913</v>
+      </c>
+      <c r="H2">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>472</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C66" si="0">CONCATENATE(D3,":",E3)</f>
+        <v>10:75900462</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>75900462</v>
+      </c>
+      <c r="F3" t="s">
+        <v>912</v>
+      </c>
+      <c r="G3" t="s">
+        <v>911</v>
+      </c>
+      <c r="H3">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>10:75924605</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>75924605</v>
+      </c>
+      <c r="F4" t="s">
+        <v>911</v>
+      </c>
+      <c r="G4" t="s">
+        <v>913</v>
+      </c>
+      <c r="H4">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>10:75892904</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>75892904</v>
+      </c>
+      <c r="F5" t="s">
+        <v>912</v>
+      </c>
+      <c r="G5" t="s">
+        <v>913</v>
+      </c>
+      <c r="H5">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>484</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>10:75936611</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>75936611</v>
+      </c>
+      <c r="F6" t="s">
+        <v>910</v>
+      </c>
+      <c r="G6" t="s">
+        <v>911</v>
+      </c>
+      <c r="H6">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>485</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>10:75939921</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>75939921</v>
+      </c>
+      <c r="F7" t="s">
+        <v>910</v>
+      </c>
+      <c r="G7" t="s">
+        <v>911</v>
+      </c>
+      <c r="H7">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44515716</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>44515716</v>
+      </c>
+      <c r="F8" t="s">
+        <v>912</v>
+      </c>
+      <c r="G8" t="s">
+        <v>913</v>
+      </c>
+      <c r="H8">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>384</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44513936</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>44513936</v>
+      </c>
+      <c r="F9" t="s">
+        <v>912</v>
+      </c>
+      <c r="G9" t="s">
+        <v>913</v>
+      </c>
+      <c r="H9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>417</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44539016</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>44539016</v>
+      </c>
+      <c r="F10" t="s">
+        <v>912</v>
+      </c>
+      <c r="G10" t="s">
+        <v>913</v>
+      </c>
+      <c r="H10">
+        <v>0.04</v>
+      </c>
+      <c r="I10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>392</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44516604</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>44516604</v>
+      </c>
+      <c r="F11" t="s">
+        <v>910</v>
+      </c>
+      <c r="G11" t="s">
+        <v>911</v>
+      </c>
+      <c r="H11">
+        <v>0.04</v>
+      </c>
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>377</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44511785</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>44511785</v>
+      </c>
+      <c r="F12" t="s">
+        <v>912</v>
+      </c>
+      <c r="G12" t="s">
+        <v>911</v>
+      </c>
+      <c r="H12">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>406</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44529320</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>44529320</v>
+      </c>
+      <c r="F13" t="s">
+        <v>912</v>
+      </c>
+      <c r="G13" t="s">
+        <v>913</v>
+      </c>
+      <c r="H13">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>398</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44518915</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>44518915</v>
+      </c>
+      <c r="F14" t="s">
+        <v>912</v>
+      </c>
+      <c r="G14" t="s">
+        <v>911</v>
+      </c>
+      <c r="H14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>383</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44513368</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>44513368</v>
+      </c>
+      <c r="F15" t="s">
+        <v>912</v>
+      </c>
+      <c r="G15" t="s">
+        <v>911</v>
+      </c>
+      <c r="H15">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>386</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44514285</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>44514285</v>
+      </c>
+      <c r="F16" t="s">
+        <v>912</v>
+      </c>
+      <c r="G16" t="s">
+        <v>913</v>
+      </c>
+      <c r="H16">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>382</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44513143</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>44513143</v>
+      </c>
+      <c r="F17" t="s">
+        <v>910</v>
+      </c>
+      <c r="G17" t="s">
+        <v>913</v>
+      </c>
+      <c r="H17">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>385</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44514106</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>44514106</v>
+      </c>
+      <c r="F18" t="s">
+        <v>912</v>
+      </c>
+      <c r="G18" t="s">
+        <v>913</v>
+      </c>
+      <c r="H18">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44514336</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>44514336</v>
+      </c>
+      <c r="F19" t="s">
+        <v>910</v>
+      </c>
+      <c r="G19" t="s">
+        <v>911</v>
+      </c>
+      <c r="H19">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>390</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44516377</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>44516377</v>
+      </c>
+      <c r="F20" t="s">
+        <v>912</v>
+      </c>
+      <c r="G20" t="s">
+        <v>913</v>
+      </c>
+      <c r="H20">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>388</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44514421</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>44514421</v>
+      </c>
+      <c r="F21" t="s">
+        <v>912</v>
+      </c>
+      <c r="G21" t="s">
+        <v>913</v>
+      </c>
+      <c r="H21">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>393</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44516610</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>44516610</v>
+      </c>
+      <c r="F22" t="s">
+        <v>910</v>
+      </c>
+      <c r="G22" t="s">
+        <v>911</v>
+      </c>
+      <c r="H22">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>397</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44518696</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>44518696</v>
+      </c>
+      <c r="F23" t="s">
+        <v>912</v>
+      </c>
+      <c r="G23" t="s">
+        <v>913</v>
+      </c>
+      <c r="H23">
+        <v>0.03</v>
+      </c>
+      <c r="I23" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>376</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44511734</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>44511734</v>
+      </c>
+      <c r="F24" t="s">
+        <v>912</v>
+      </c>
+      <c r="G24" t="s">
+        <v>913</v>
+      </c>
+      <c r="H24">
+        <v>2.3E-2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>375</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44511715</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>44511715</v>
+      </c>
+      <c r="F25" t="s">
+        <v>912</v>
+      </c>
+      <c r="G25" t="s">
+        <v>913</v>
+      </c>
+      <c r="H25">
+        <v>2.3E-2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>379</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44511905</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>44511905</v>
+      </c>
+      <c r="F26" t="s">
+        <v>912</v>
+      </c>
+      <c r="G26" t="s">
+        <v>911</v>
+      </c>
+      <c r="H26">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>410</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44535833</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>44535833</v>
+      </c>
+      <c r="F27" t="s">
+        <v>911</v>
+      </c>
+      <c r="G27" t="s">
+        <v>913</v>
+      </c>
+      <c r="H27">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I27" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>396</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44518652</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <v>44518652</v>
+      </c>
+      <c r="F28" t="s">
+        <v>912</v>
+      </c>
+      <c r="G28" t="s">
+        <v>913</v>
+      </c>
+      <c r="H28">
+        <v>0.02</v>
+      </c>
+      <c r="I28" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>394</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44517790</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>44517790</v>
+      </c>
+      <c r="F29" t="s">
+        <v>912</v>
+      </c>
+      <c r="G29" t="s">
+        <v>913</v>
+      </c>
+      <c r="H29">
+        <v>0.02</v>
+      </c>
+      <c r="I29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>371</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44509828</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>44509828</v>
+      </c>
+      <c r="F30" t="s">
+        <v>911</v>
+      </c>
+      <c r="G30" t="s">
+        <v>913</v>
+      </c>
+      <c r="H30">
+        <v>1.9E-2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>391</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44516421</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>44516421</v>
+      </c>
+      <c r="F31" t="s">
+        <v>912</v>
+      </c>
+      <c r="G31" t="s">
+        <v>913</v>
+      </c>
+      <c r="H31">
+        <v>1.4E-2</v>
+      </c>
+      <c r="I31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>412</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44537423</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>44537423</v>
+      </c>
+      <c r="F32" t="s">
+        <v>911</v>
+      </c>
+      <c r="G32" t="s">
+        <v>913</v>
+      </c>
+      <c r="H32">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I32" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>415</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44538672</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>44538672</v>
+      </c>
+      <c r="F33" t="s">
+        <v>912</v>
+      </c>
+      <c r="G33" t="s">
+        <v>913</v>
+      </c>
+      <c r="H33">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I33" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>378</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44511815</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>44511815</v>
+      </c>
+      <c r="F34" t="s">
+        <v>911</v>
+      </c>
+      <c r="G34" t="s">
+        <v>913</v>
+      </c>
+      <c r="H34">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I34" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>368</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44508242</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>44508242</v>
+      </c>
+      <c r="F35" t="s">
+        <v>910</v>
+      </c>
+      <c r="G35" t="s">
+        <v>911</v>
+      </c>
+      <c r="H35">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I35" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>369</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44509338</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
+      <c r="E36">
+        <v>44509338</v>
+      </c>
+      <c r="F36" t="s">
+        <v>912</v>
+      </c>
+      <c r="G36" t="s">
+        <v>913</v>
+      </c>
+      <c r="H36">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I36" t="s">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>370</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44509620</v>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>44509620</v>
+      </c>
+      <c r="F37" t="s">
+        <v>911</v>
+      </c>
+      <c r="G37" t="s">
+        <v>913</v>
+      </c>
+      <c r="H37">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I37" t="s">
+        <v>0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>416</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44538921</v>
+      </c>
+      <c r="D38">
+        <v>10</v>
+      </c>
+      <c r="E38">
+        <v>44538921</v>
+      </c>
+      <c r="F38" t="s">
+        <v>910</v>
+      </c>
+      <c r="G38" t="s">
+        <v>911</v>
+      </c>
+      <c r="H38">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I38" t="s">
+        <v>0</v>
+      </c>
+      <c r="J38" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>359</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44501946</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>44501946</v>
+      </c>
+      <c r="F39" t="s">
+        <v>912</v>
+      </c>
+      <c r="G39" t="s">
+        <v>913</v>
+      </c>
+      <c r="H39">
+        <v>0.01</v>
+      </c>
+      <c r="I39" t="s">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>380</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44512570</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>44512570</v>
+      </c>
+      <c r="F40" t="s">
+        <v>912</v>
+      </c>
+      <c r="G40" t="s">
+        <v>913</v>
+      </c>
+      <c r="H40">
+        <v>0.01</v>
+      </c>
+      <c r="I40" t="s">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>968</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44535508</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41">
+        <v>44535508</v>
+      </c>
+      <c r="F41" t="s">
+        <v>912</v>
+      </c>
+      <c r="G41" t="s">
+        <v>913</v>
+      </c>
+      <c r="H41">
+        <v>0.01</v>
+      </c>
+      <c r="I41" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>413</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44537706</v>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>44537706</v>
+      </c>
+      <c r="F42" t="s">
+        <v>912</v>
+      </c>
+      <c r="G42" t="s">
+        <v>913</v>
+      </c>
+      <c r="H42">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I42" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>348</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44495365</v>
+      </c>
+      <c r="D43">
+        <v>10</v>
+      </c>
+      <c r="E43">
+        <v>44495365</v>
+      </c>
+      <c r="F43" t="s">
+        <v>910</v>
+      </c>
+      <c r="G43" t="s">
+        <v>911</v>
+      </c>
+      <c r="H43">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>363</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44505391</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+      <c r="E44">
+        <v>44505391</v>
+      </c>
+      <c r="F44" t="s">
+        <v>910</v>
+      </c>
+      <c r="G44" t="s">
+        <v>913</v>
+      </c>
+      <c r="H44">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I44" t="s">
+        <v>0</v>
+      </c>
+      <c r="J44" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>365</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44505534</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45">
+        <v>44505534</v>
+      </c>
+      <c r="F45" t="s">
+        <v>912</v>
+      </c>
+      <c r="G45" t="s">
+        <v>913</v>
+      </c>
+      <c r="H45">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I45" t="s">
+        <v>0</v>
+      </c>
+      <c r="J45" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>403</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44527590</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+      <c r="E46">
+        <v>44527590</v>
+      </c>
+      <c r="F46" t="s">
+        <v>910</v>
+      </c>
+      <c r="G46" t="s">
+        <v>911</v>
+      </c>
+      <c r="H46">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I46" t="s">
+        <v>0</v>
+      </c>
+      <c r="J46" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>360</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44504359</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+      <c r="E47">
+        <v>44504359</v>
+      </c>
+      <c r="F47" t="s">
+        <v>910</v>
+      </c>
+      <c r="G47" t="s">
+        <v>911</v>
+      </c>
+      <c r="H47">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I47" t="s">
+        <v>0</v>
+      </c>
+      <c r="J47" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>401</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44523504</v>
+      </c>
+      <c r="D48">
+        <v>10</v>
+      </c>
+      <c r="E48">
+        <v>44523504</v>
+      </c>
+      <c r="F48" t="s">
+        <v>910</v>
+      </c>
+      <c r="G48" t="s">
+        <v>911</v>
+      </c>
+      <c r="H48">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I48" t="s">
+        <v>0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>362</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44505025</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+      <c r="E49">
+        <v>44505025</v>
+      </c>
+      <c r="F49" t="s">
+        <v>912</v>
+      </c>
+      <c r="G49" t="s">
+        <v>913</v>
+      </c>
+      <c r="H49">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>364</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44505466</v>
+      </c>
+      <c r="D50">
+        <v>10</v>
+      </c>
+      <c r="E50">
+        <v>44505466</v>
+      </c>
+      <c r="F50" t="s">
+        <v>910</v>
+      </c>
+      <c r="G50" t="s">
+        <v>913</v>
+      </c>
+      <c r="H50">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I50" t="s">
+        <v>0</v>
+      </c>
+      <c r="J50" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>350</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44496985</v>
+      </c>
+      <c r="D51">
+        <v>10</v>
+      </c>
+      <c r="E51">
+        <v>44496985</v>
+      </c>
+      <c r="F51" t="s">
+        <v>910</v>
+      </c>
+      <c r="G51" t="s">
+        <v>911</v>
+      </c>
+      <c r="H51">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I51" t="s">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>402</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44527132</v>
+      </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+      <c r="E52">
+        <v>44527132</v>
+      </c>
+      <c r="F52" t="s">
+        <v>910</v>
+      </c>
+      <c r="G52" t="s">
+        <v>911</v>
+      </c>
+      <c r="H52">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>357</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44501266</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>44501266</v>
+      </c>
+      <c r="F53" t="s">
+        <v>910</v>
+      </c>
+      <c r="G53" t="s">
+        <v>911</v>
+      </c>
+      <c r="H53">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I53" t="s">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>969</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44494546</v>
+      </c>
+      <c r="D54">
+        <v>10</v>
+      </c>
+      <c r="E54">
+        <v>44494546</v>
+      </c>
+      <c r="F54" t="s">
+        <v>912</v>
+      </c>
+      <c r="G54" t="s">
+        <v>913</v>
+      </c>
+      <c r="H54">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I54" t="s">
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>344</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44490854</v>
+      </c>
+      <c r="D55">
+        <v>10</v>
+      </c>
+      <c r="E55">
+        <v>44490854</v>
+      </c>
+      <c r="F55" t="s">
+        <v>912</v>
+      </c>
+      <c r="G55" t="s">
+        <v>913</v>
+      </c>
+      <c r="H55">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I55" t="s">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>418</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>10:44539913</v>
+      </c>
+      <c r="D56">
+        <v>10</v>
+      </c>
+      <c r="E56">
+        <v>44539913</v>
+      </c>
+      <c r="F56" t="s">
+        <v>910</v>
+      </c>
+      <c r="G56" t="s">
+        <v>913</v>
+      </c>
+      <c r="H56">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I56" t="s">
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>595</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>12:4486618</v>
+      </c>
+      <c r="D57">
+        <v>12</v>
+      </c>
+      <c r="E57">
+        <v>4486618</v>
+      </c>
+      <c r="F57" t="s">
+        <v>912</v>
+      </c>
+      <c r="G57" t="s">
+        <v>913</v>
+      </c>
+      <c r="H57">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="I57" t="s">
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>7:45960645</v>
+      </c>
+      <c r="D58">
+        <v>7</v>
+      </c>
+      <c r="E58">
+        <v>45960645</v>
+      </c>
+      <c r="F58" t="s">
+        <v>911</v>
+      </c>
+      <c r="G58" t="s">
+        <v>913</v>
+      </c>
+      <c r="H58">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="I58" t="s">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>7:45978060</v>
+      </c>
+      <c r="D59">
+        <v>7</v>
+      </c>
+      <c r="E59">
+        <v>45978060</v>
+      </c>
+      <c r="F59" t="s">
+        <v>912</v>
+      </c>
+      <c r="G59" t="s">
+        <v>913</v>
+      </c>
+      <c r="H59">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I59" t="s">
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>7:45970037</v>
+      </c>
+      <c r="D60">
+        <v>7</v>
+      </c>
+      <c r="E60">
+        <v>45970037</v>
+      </c>
+      <c r="F60" t="s">
+        <v>912</v>
+      </c>
+      <c r="G60" t="s">
+        <v>913</v>
+      </c>
+      <c r="H60">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I60" t="s">
+        <v>0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>86</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>7:45963114</v>
+      </c>
+      <c r="D61">
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <v>45963114</v>
+      </c>
+      <c r="F61" t="s">
+        <v>910</v>
+      </c>
+      <c r="G61" t="s">
+        <v>911</v>
+      </c>
+      <c r="H61">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I61" t="s">
+        <v>0</v>
+      </c>
+      <c r="J61" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>7:45980751</v>
+      </c>
+      <c r="D62">
+        <v>7</v>
+      </c>
+      <c r="E62">
+        <v>45980751</v>
+      </c>
+      <c r="F62" t="s">
+        <v>910</v>
+      </c>
+      <c r="G62" t="s">
+        <v>913</v>
+      </c>
+      <c r="H62">
+        <v>3.1E-2</v>
+      </c>
+      <c r="I62" t="s">
+        <v>0</v>
+      </c>
+      <c r="J62" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>7:45974375</v>
+      </c>
+      <c r="D63">
+        <v>7</v>
+      </c>
+      <c r="E63">
+        <v>45974375</v>
+      </c>
+      <c r="F63" t="s">
+        <v>910</v>
+      </c>
+      <c r="G63" t="s">
+        <v>911</v>
+      </c>
+      <c r="H63">
+        <v>2.3E-2</v>
+      </c>
+      <c r="I63" t="s">
+        <v>0</v>
+      </c>
+      <c r="J63" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>7:45978059</v>
+      </c>
+      <c r="D64">
+        <v>7</v>
+      </c>
+      <c r="E64">
+        <v>45978059</v>
+      </c>
+      <c r="F64" t="s">
+        <v>910</v>
+      </c>
+      <c r="G64" t="s">
+        <v>911</v>
+      </c>
+      <c r="H64">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I64" t="s">
+        <v>0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>7:45977352</v>
+      </c>
+      <c r="D65">
+        <v>7</v>
+      </c>
+      <c r="E65">
+        <v>45977352</v>
+      </c>
+      <c r="F65" t="s">
+        <v>912</v>
+      </c>
+      <c r="G65" t="s">
+        <v>913</v>
+      </c>
+      <c r="H65">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I65" t="s">
+        <v>0</v>
+      </c>
+      <c r="J65" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>90</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>7:45972977</v>
+      </c>
+      <c r="D66">
+        <v>7</v>
+      </c>
+      <c r="E66">
+        <v>45972977</v>
+      </c>
+      <c r="F66" t="s">
+        <v>912</v>
+      </c>
+      <c r="G66" t="s">
+        <v>913</v>
+      </c>
+      <c r="H66">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I66" t="s">
+        <v>0</v>
+      </c>
+      <c r="J66" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" ref="C67:C104" si="1">CONCATENATE(D67,":",E67)</f>
+        <v>6:132095002</v>
+      </c>
+      <c r="D67">
+        <v>6</v>
+      </c>
+      <c r="E67">
+        <v>132095002</v>
+      </c>
+      <c r="F67" t="s">
+        <v>910</v>
+      </c>
+      <c r="G67" t="s">
+        <v>911</v>
+      </c>
+      <c r="H67">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I67" t="s">
+        <v>0</v>
+      </c>
+      <c r="J67" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>6:132093691</v>
+      </c>
+      <c r="D68">
+        <v>6</v>
+      </c>
+      <c r="E68">
+        <v>132093691</v>
+      </c>
+      <c r="F68" t="s">
+        <v>912</v>
+      </c>
+      <c r="G68" t="s">
+        <v>911</v>
+      </c>
+      <c r="H68">
+        <v>0.193</v>
+      </c>
+      <c r="I68" t="s">
+        <v>0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>6:132089007</v>
+      </c>
+      <c r="D69">
+        <v>6</v>
+      </c>
+      <c r="E69">
+        <v>132089007</v>
+      </c>
+      <c r="F69" t="s">
+        <v>910</v>
+      </c>
+      <c r="G69" t="s">
+        <v>911</v>
+      </c>
+      <c r="H69">
+        <v>0.192</v>
+      </c>
+      <c r="I69" t="s">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>310</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>9:22124744</v>
+      </c>
+      <c r="D70">
+        <v>9</v>
+      </c>
+      <c r="E70">
+        <v>22124744</v>
+      </c>
+      <c r="F70" t="s">
+        <v>911</v>
+      </c>
+      <c r="G70" t="s">
+        <v>913</v>
+      </c>
+      <c r="H70">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="I70" t="s">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>308</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>9:22124504</v>
+      </c>
+      <c r="D71">
+        <v>9</v>
+      </c>
+      <c r="E71">
+        <v>22124504</v>
+      </c>
+      <c r="F71" t="s">
+        <v>912</v>
+      </c>
+      <c r="G71" t="s">
+        <v>910</v>
+      </c>
+      <c r="H71">
+        <v>0.35</v>
+      </c>
+      <c r="I71" t="s">
+        <v>0</v>
+      </c>
+      <c r="J71" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>275</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>9:22103341</v>
+      </c>
+      <c r="D72">
+        <v>9</v>
+      </c>
+      <c r="E72">
+        <v>22103341</v>
+      </c>
+      <c r="F72" t="s">
+        <v>910</v>
+      </c>
+      <c r="G72" t="s">
+        <v>913</v>
+      </c>
+      <c r="H72">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I72" t="s">
+        <v>0</v>
+      </c>
+      <c r="J72" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>807</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79123946</v>
+      </c>
+      <c r="D73">
+        <v>15</v>
+      </c>
+      <c r="E73">
+        <v>79123946</v>
+      </c>
+      <c r="F73" t="s">
+        <v>910</v>
+      </c>
+      <c r="G73" t="s">
+        <v>913</v>
+      </c>
+      <c r="H73">
+        <v>0.122</v>
+      </c>
+      <c r="I73" t="s">
+        <v>0</v>
+      </c>
+      <c r="J73" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>798</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79123338</v>
+      </c>
+      <c r="D74">
+        <v>15</v>
+      </c>
+      <c r="E74">
+        <v>79123338</v>
+      </c>
+      <c r="F74" t="s">
+        <v>911</v>
+      </c>
+      <c r="G74" t="s">
+        <v>913</v>
+      </c>
+      <c r="H74">
+        <v>0.106</v>
+      </c>
+      <c r="I74" t="s">
+        <v>0</v>
+      </c>
+      <c r="J74" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>801</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79123509</v>
+      </c>
+      <c r="D75">
+        <v>15</v>
+      </c>
+      <c r="E75">
+        <v>79123509</v>
+      </c>
+      <c r="F75" t="s">
+        <v>910</v>
+      </c>
+      <c r="G75" t="s">
+        <v>913</v>
+      </c>
+      <c r="H75">
+        <v>0.106</v>
+      </c>
+      <c r="I75" t="s">
+        <v>0</v>
+      </c>
+      <c r="J75" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>797</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79123054</v>
+      </c>
+      <c r="D76">
+        <v>15</v>
+      </c>
+      <c r="E76">
+        <v>79123054</v>
+      </c>
+      <c r="F76" t="s">
+        <v>910</v>
+      </c>
+      <c r="G76" t="s">
+        <v>911</v>
+      </c>
+      <c r="H76">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I76" t="s">
+        <v>0</v>
+      </c>
+      <c r="J76" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>804</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79123753</v>
+      </c>
+      <c r="D77">
+        <v>15</v>
+      </c>
+      <c r="E77">
+        <v>79123753</v>
+      </c>
+      <c r="F77" t="s">
+        <v>910</v>
+      </c>
+      <c r="G77" t="s">
+        <v>911</v>
+      </c>
+      <c r="H77">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="I77" t="s">
+        <v>0</v>
+      </c>
+      <c r="J77" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>805</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79123779</v>
+      </c>
+      <c r="D78">
+        <v>15</v>
+      </c>
+      <c r="E78">
+        <v>79123779</v>
+      </c>
+      <c r="F78" t="s">
+        <v>910</v>
+      </c>
+      <c r="G78" t="s">
+        <v>911</v>
+      </c>
+      <c r="H78">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="I78" t="s">
+        <v>0</v>
+      </c>
+      <c r="J78" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>803</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79123631</v>
+      </c>
+      <c r="D79">
+        <v>15</v>
+      </c>
+      <c r="E79">
+        <v>79123631</v>
+      </c>
+      <c r="F79" t="s">
+        <v>910</v>
+      </c>
+      <c r="G79" t="s">
+        <v>911</v>
+      </c>
+      <c r="H79">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="I79" t="s">
+        <v>0</v>
+      </c>
+      <c r="J79" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>800</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79123505</v>
+      </c>
+      <c r="D80">
+        <v>15</v>
+      </c>
+      <c r="E80">
+        <v>79123505</v>
+      </c>
+      <c r="F80" t="s">
+        <v>912</v>
+      </c>
+      <c r="G80" t="s">
+        <v>913</v>
+      </c>
+      <c r="H80">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I80" t="s">
+        <v>0</v>
+      </c>
+      <c r="J80" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>799</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79123396</v>
+      </c>
+      <c r="D81">
+        <v>15</v>
+      </c>
+      <c r="E81">
+        <v>79123396</v>
+      </c>
+      <c r="F81" t="s">
+        <v>911</v>
+      </c>
+      <c r="G81" t="s">
+        <v>913</v>
+      </c>
+      <c r="H81">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="I81" t="s">
+        <v>0</v>
+      </c>
+      <c r="J81" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>769</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79114453</v>
+      </c>
+      <c r="D82">
+        <v>15</v>
+      </c>
+      <c r="E82">
+        <v>79114453</v>
+      </c>
+      <c r="F82" t="s">
+        <v>910</v>
+      </c>
+      <c r="G82" t="s">
+        <v>911</v>
+      </c>
+      <c r="H82">
+        <v>0.06</v>
+      </c>
+      <c r="I82" t="s">
+        <v>0</v>
+      </c>
+      <c r="J82" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>792</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>15:79121776</v>
+      </c>
+      <c r="D83">
+        <v>15</v>
+      </c>
+      <c r="E83">
+        <v>79121776</v>
+      </c>
+      <c r="F83" t="s">
+        <v>910</v>
+      </c>
+      <c r="G83" t="s">
+        <v>911</v>
+      </c>
+      <c r="H83">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="I83" t="s">
+        <v>0</v>
+      </c>
+      <c r="J83" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>902</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>19:45412079</v>
+      </c>
+      <c r="D84">
+        <v>19</v>
+      </c>
+      <c r="E84">
+        <v>45412079</v>
+      </c>
+      <c r="F84" t="s">
+        <v>910</v>
+      </c>
+      <c r="G84" t="s">
+        <v>911</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>0</v>
+      </c>
+      <c r="J84" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>6:12903957</v>
+      </c>
+      <c r="D85">
+        <v>6</v>
+      </c>
+      <c r="E85">
+        <v>12903957</v>
+      </c>
+      <c r="F85" t="s">
+        <v>912</v>
+      </c>
+      <c r="G85" t="s">
+        <v>913</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85" t="s">
+        <v>0</v>
+      </c>
+      <c r="J85" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>604</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>13:111049623</v>
+      </c>
+      <c r="D86">
+        <v>13</v>
+      </c>
+      <c r="E86">
+        <v>111049623</v>
+      </c>
+      <c r="F86" t="s">
+        <v>910</v>
+      </c>
+      <c r="G86" t="s">
+        <v>911</v>
+      </c>
+      <c r="H86">
+        <v>0.999</v>
+      </c>
+      <c r="I86" t="s">
+        <v>0</v>
+      </c>
+      <c r="J86" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>439</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63836088</v>
+      </c>
+      <c r="D87">
+        <v>10</v>
+      </c>
+      <c r="E87">
+        <v>63836088</v>
+      </c>
+      <c r="F87" t="s">
+        <v>910</v>
+      </c>
+      <c r="G87" t="s">
+        <v>911</v>
+      </c>
+      <c r="H87">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="I87" t="s">
+        <v>0</v>
+      </c>
+      <c r="J87" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>436</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63835015</v>
+      </c>
+      <c r="D88">
+        <v>10</v>
+      </c>
+      <c r="E88">
+        <v>63835015</v>
+      </c>
+      <c r="F88" t="s">
+        <v>912</v>
+      </c>
+      <c r="G88" t="s">
+        <v>911</v>
+      </c>
+      <c r="H88">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="I88" t="s">
+        <v>0</v>
+      </c>
+      <c r="J88" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>437</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63835193</v>
+      </c>
+      <c r="D89">
+        <v>10</v>
+      </c>
+      <c r="E89">
+        <v>63835193</v>
+      </c>
+      <c r="F89" t="s">
+        <v>912</v>
+      </c>
+      <c r="G89" t="s">
+        <v>913</v>
+      </c>
+      <c r="H89">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="I89" t="s">
+        <v>0</v>
+      </c>
+      <c r="J89" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>438</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63835692</v>
+      </c>
+      <c r="D90">
+        <v>10</v>
+      </c>
+      <c r="E90">
+        <v>63835692</v>
+      </c>
+      <c r="F90" t="s">
+        <v>912</v>
+      </c>
+      <c r="G90" t="s">
+        <v>913</v>
+      </c>
+      <c r="H90">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="I90" t="s">
+        <v>0</v>
+      </c>
+      <c r="J90" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>428</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63830984</v>
+      </c>
+      <c r="D91">
+        <v>10</v>
+      </c>
+      <c r="E91">
+        <v>63830984</v>
+      </c>
+      <c r="F91" t="s">
+        <v>912</v>
+      </c>
+      <c r="G91" t="s">
+        <v>913</v>
+      </c>
+      <c r="H91">
+        <v>7.8E-2</v>
+      </c>
+      <c r="I91" t="s">
+        <v>0</v>
+      </c>
+      <c r="J91" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>426</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63828879</v>
+      </c>
+      <c r="D92">
+        <v>10</v>
+      </c>
+      <c r="E92">
+        <v>63828879</v>
+      </c>
+      <c r="F92" t="s">
+        <v>912</v>
+      </c>
+      <c r="G92" t="s">
+        <v>910</v>
+      </c>
+      <c r="H92">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I92" t="s">
+        <v>0</v>
+      </c>
+      <c r="J92" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>434</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63834048</v>
+      </c>
+      <c r="D93">
+        <v>10</v>
+      </c>
+      <c r="E93">
+        <v>63834048</v>
+      </c>
+      <c r="F93" t="s">
+        <v>910</v>
+      </c>
+      <c r="G93" t="s">
+        <v>911</v>
+      </c>
+      <c r="H93">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="I93" t="s">
+        <v>0</v>
+      </c>
+      <c r="J93" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>429</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63831501</v>
+      </c>
+      <c r="D94">
+        <v>10</v>
+      </c>
+      <c r="E94">
+        <v>63831501</v>
+      </c>
+      <c r="F94" t="s">
+        <v>910</v>
+      </c>
+      <c r="G94" t="s">
+        <v>913</v>
+      </c>
+      <c r="H94">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="I94" t="s">
+        <v>0</v>
+      </c>
+      <c r="J94" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>433</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63832898</v>
+      </c>
+      <c r="D95">
+        <v>10</v>
+      </c>
+      <c r="E95">
+        <v>63832898</v>
+      </c>
+      <c r="F95" t="s">
+        <v>912</v>
+      </c>
+      <c r="G95" t="s">
+        <v>913</v>
+      </c>
+      <c r="H95">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I95" t="s">
+        <v>0</v>
+      </c>
+      <c r="J95" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>430</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63831928</v>
+      </c>
+      <c r="D96">
+        <v>10</v>
+      </c>
+      <c r="E96">
+        <v>63831928</v>
+      </c>
+      <c r="F96" t="s">
+        <v>912</v>
+      </c>
+      <c r="G96" t="s">
+        <v>913</v>
+      </c>
+      <c r="H96">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I96" t="s">
+        <v>0</v>
+      </c>
+      <c r="J96" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>427</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63830286</v>
+      </c>
+      <c r="D97">
+        <v>10</v>
+      </c>
+      <c r="E97">
+        <v>63830286</v>
+      </c>
+      <c r="F97" t="s">
+        <v>910</v>
+      </c>
+      <c r="G97" t="s">
+        <v>911</v>
+      </c>
+      <c r="H97">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I97" t="s">
+        <v>0</v>
+      </c>
+      <c r="J97" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>440</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63837006</v>
+      </c>
+      <c r="D98">
+        <v>10</v>
+      </c>
+      <c r="E98">
+        <v>63837006</v>
+      </c>
+      <c r="F98" t="s">
+        <v>912</v>
+      </c>
+      <c r="G98" t="s">
+        <v>913</v>
+      </c>
+      <c r="H98">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I98" t="s">
+        <v>0</v>
+      </c>
+      <c r="J98" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>441</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63837016</v>
+      </c>
+      <c r="D99">
+        <v>10</v>
+      </c>
+      <c r="E99">
+        <v>63837016</v>
+      </c>
+      <c r="F99" t="s">
+        <v>910</v>
+      </c>
+      <c r="G99" t="s">
+        <v>911</v>
+      </c>
+      <c r="H99">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I99" t="s">
+        <v>0</v>
+      </c>
+      <c r="J99" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>442</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63837255</v>
+      </c>
+      <c r="D100">
+        <v>10</v>
+      </c>
+      <c r="E100">
+        <v>63837255</v>
+      </c>
+      <c r="F100" t="s">
+        <v>912</v>
+      </c>
+      <c r="G100" t="s">
+        <v>913</v>
+      </c>
+      <c r="H100">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I100" t="s">
+        <v>0</v>
+      </c>
+      <c r="J100" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>979</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63818425</v>
+      </c>
+      <c r="D101">
+        <v>10</v>
+      </c>
+      <c r="E101">
+        <v>63818425</v>
+      </c>
+      <c r="F101" t="s">
+        <v>912</v>
+      </c>
+      <c r="G101" t="s">
+        <v>910</v>
+      </c>
+      <c r="H101">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I101" t="s">
+        <v>0</v>
+      </c>
+      <c r="J101" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>446</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63840687</v>
+      </c>
+      <c r="D102">
+        <v>10</v>
+      </c>
+      <c r="E102">
+        <v>63840687</v>
+      </c>
+      <c r="F102" t="s">
+        <v>910</v>
+      </c>
+      <c r="G102" t="s">
+        <v>913</v>
+      </c>
+      <c r="H102">
+        <v>0.02</v>
+      </c>
+      <c r="I102" t="s">
+        <v>0</v>
+      </c>
+      <c r="J102" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>980</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63818424</v>
+      </c>
+      <c r="D103">
+        <v>10</v>
+      </c>
+      <c r="E103">
+        <v>63818424</v>
+      </c>
+      <c r="F103" t="s">
+        <v>910</v>
+      </c>
+      <c r="G103" t="s">
+        <v>913</v>
+      </c>
+      <c r="H103">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="I103" t="s">
+        <v>0</v>
+      </c>
+      <c r="J103" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>445</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="1"/>
+        <v>10:63839417</v>
+      </c>
+      <c r="D104">
+        <v>10</v>
+      </c>
+      <c r="E104">
+        <v>63839417</v>
+      </c>
+      <c r="F104" t="s">
+        <v>910</v>
+      </c>
+      <c r="G104" t="s">
+        <v>911</v>
+      </c>
+      <c r="H104">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I104" t="s">
+        <v>0</v>
+      </c>
+      <c r="J104" t="s">
+        <v>978</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>